<commit_message>
Update a little more
</commit_message>
<xml_diff>
--- a/HITEL/list.xlsx
+++ b/HITEL/list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Viola15_font\HITEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069F500A-7074-421E-B33F-475E3615C344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6433EA4-EE05-4C64-9417-40269C21FA9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ECBBBA91-6ACC-4411-8119-0B98102DD867}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="577">
   <si>
     <t>ad24.han</t>
   </si>
@@ -1963,6 +1963,26 @@
   </si>
   <si>
     <t>hm.spc</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>명조같은 느낌</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>손글씨</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>둥금</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>얇음</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>yun.ksg</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -2389,8 +2409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7EE061E-4DF6-4129-B2C9-943A90EE26B5}">
   <dimension ref="A1:L158"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2970,7 +2990,7 @@
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
         <f t="shared" si="0"/>
-        <v>dokkebi_han.py eng\ad24.eng han\ad24.han ksg\roman.ksg spc\sys.spc</v>
+        <v>dokkebi_han.py eng\ad24.eng han\ad24.han ksg\yun.ksg spc\sys.spc</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>315</v>
@@ -2993,7 +3013,7 @@
         <v>김윤수</v>
       </c>
       <c r="I21" t="s">
-        <v>522</v>
+        <v>576</v>
       </c>
       <c r="L21" t="s">
         <v>551</v>
@@ -3002,7 +3022,7 @@
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
         <f t="shared" si="0"/>
-        <v>dokkebi_han.py eng\ad24_10.eng han\ad24.han ksg\roman.ksg spc\sys.spc</v>
+        <v>dokkebi_han.py eng\ad24_10.eng han\ad24.han ksg\yun.ksg spc\sys.spc</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>315</v>
@@ -3025,7 +3045,7 @@
         <v>김윤수</v>
       </c>
       <c r="I22" t="s">
-        <v>522</v>
+        <v>576</v>
       </c>
       <c r="L22" t="s">
         <v>551</v>
@@ -7862,15 +7882,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{770541BF-A55C-4418-BBA8-17C60E69C320}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>539</v>
       </c>
@@ -7878,7 +7898,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>540</v>
       </c>
@@ -7886,7 +7906,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>541</v>
       </c>
@@ -7894,7 +7914,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>542</v>
       </c>
@@ -7902,7 +7922,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>543</v>
       </c>
@@ -7910,7 +7930,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>544</v>
       </c>
@@ -7921,7 +7941,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>545</v>
       </c>
@@ -7931,8 +7951,11 @@
       <c r="C7" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>546</v>
       </c>
@@ -7943,7 +7966,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>547</v>
       </c>
@@ -7951,7 +7974,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>548</v>
       </c>
@@ -7959,15 +7982,18 @@
         <v>557</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>549</v>
       </c>
       <c r="B11" t="s">
         <v>560</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>550</v>
       </c>
@@ -7977,8 +8003,11 @@
       <c r="C12" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>551</v>
       </c>
@@ -7986,7 +8015,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>552</v>
       </c>
@@ -7997,12 +8026,15 @@
         <v>222</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>553</v>
       </c>
       <c r="B15" t="s">
         <v>566</v>
+      </c>
+      <c r="F15" t="s">
+        <v>573</v>
       </c>
     </row>
   </sheetData>

</xml_diff>